<commit_message>
Reports file name changed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestLinks.xlsx
+++ b/src/test/resources/TestLinks.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
-  <si>
-    <t>Links</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -35,40 +32,7 @@
     <t>Test Case</t>
   </si>
   <si>
-    <t>Start Time</t>
-  </si>
-  <si>
-    <t>End Time</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>TC_001</t>
-  </si>
-  <si>
-    <t>With Valid Data</t>
-  </si>
-  <si>
-    <t>Data 1</t>
-  </si>
-  <si>
-    <t>29-08-2020-15-00-03</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>TC_002</t>
-  </si>
-  <si>
-    <t>TC_003</t>
-  </si>
-  <si>
-    <t>TC_004</t>
-  </si>
-  <si>
-    <t>TC_005</t>
+    <t>Pges</t>
   </si>
 </sst>
 </file>
@@ -118,10 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" activeCellId="1" sqref="J13 J13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,124 +380,15 @@
     <col min="5" max="5" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>